<commit_message>
fasteners folder, BOM for battery pack
</commit_message>
<xml_diff>
--- a/BOM/BatteryHolder/BatHolder.xlsx
+++ b/BOM/BatteryHolder/BatHolder.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\LongboardMarkII\BOM\BatteryHolder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LongboardMarkII\BOM\BatteryHolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Item Name</t>
   </si>
@@ -47,15 +47,9 @@
     <t>Quanity Units</t>
   </si>
   <si>
-    <t>Yards</t>
-  </si>
-  <si>
     <t>Item Desc</t>
   </si>
   <si>
-    <t>.012" thick 50" Width</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -71,13 +65,46 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>All Carbon</t>
-  </si>
-  <si>
-    <t>6'x3" 3/8 Aluminum</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/#8975k91/=199we9i</t>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>6'x3/8"x3/8" Aluminum</t>
+  </si>
+  <si>
+    <t>6'x3"x3/8" Aluminum</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#8975k617/=19bnny9</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#9008k78/=19bno32</t>
+  </si>
+  <si>
+    <t>feet</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>6-32 thread</t>
+  </si>
+  <si>
+    <t>Black Oxide Screw 1.75"</t>
+  </si>
+  <si>
+    <t>Aluminum spacers 5/16"</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#91251a158/=19bnq2t</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#8585k205/=19bof2z</t>
+  </si>
+  <si>
+    <t>polycarbonate tube</t>
+  </si>
+  <si>
+    <t>1.125" ID 1.25" OD</t>
   </si>
 </sst>
 </file>
@@ -125,10 +152,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -447,7 +475,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,9 +490,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -484,46 +509,44 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E2">
-        <v>47</v>
+        <f>47.25/6</f>
+        <v>7.875</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -536,23 +559,192 @@
       </c>
       <c r="L2">
         <f>E2*F2*I2*(1+J2)</f>
-        <v>50.760000000000005</v>
+        <v>51.03</v>
+      </c>
+      <c r="M2">
+        <f>L2+K2</f>
+        <v>51.03</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D3" s="2"/>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <f>6.81/6</f>
+        <v>1.135</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.08</v>
+      </c>
+      <c r="K3">
+        <v>33</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L7" si="0">E3*F3*I3*(1+J3)</f>
+        <v>7.3548000000000009</v>
+      </c>
+      <c r="M3">
+        <f>M2+L3</f>
+        <v>58.384799999999998</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D4" s="2"/>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F4">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.08</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>8.1648000000000014</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M7" si="1">M3+L4</f>
+        <v>66.549599999999998</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D5" s="2"/>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <f>7.1/50</f>
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.08</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>74.217600000000004</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D6" s="2"/>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3">
+        <f>19.89/8</f>
+        <v>2.4862500000000001</v>
+      </c>
+      <c r="F6">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0.08</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>42.962400000000002</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>117.18</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D7" s="2"/>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0.08</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>117.18</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D8" s="2"/>
@@ -568,10 +760,6 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
-      <c r="M14">
-        <f>SUM(L2:L14)</f>
-        <v>50.760000000000005</v>
-      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D16" s="2"/>
@@ -613,9 +801,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" location="8975k91/=199we9i" xr:uid="{18A7086B-4922-4F21-A85F-453934409742}"/>
+    <hyperlink ref="D2" r:id="rId1" location="8975k617/=19bnny9" xr:uid="{18A7086B-4922-4F21-A85F-453934409742}"/>
+    <hyperlink ref="D3" r:id="rId2" location="9008k78/=19bno32" xr:uid="{0903AB3E-4941-460C-8B26-6317F3CB18E0}"/>
+    <hyperlink ref="D4" r:id="rId3" location="9008k78/=19bno32" xr:uid="{3E248846-5CE3-470E-A5E7-5ED38B41D492}"/>
+    <hyperlink ref="D5" r:id="rId4" location="91251a158/=19bnq2t" xr:uid="{6CF9EFF7-6077-47C6-B406-2905E3FA64D1}"/>
+    <hyperlink ref="D6" r:id="rId5" location="8585k205/=19bof2z" xr:uid="{04AB373F-6377-4008-A03D-91B129D7D564}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Compiled Bat Holder BOM
</commit_message>
<xml_diff>
--- a/BOM/BatteryHolder/BatHolder.xlsx
+++ b/BOM/BatteryHolder/BatHolder.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Item Name</t>
   </si>
@@ -105,6 +105,78 @@
   </si>
   <si>
     <t>1.125" ID 1.25" OD</t>
+  </si>
+  <si>
+    <t>aluminum tube 1.25"OD</t>
+  </si>
+  <si>
+    <t>1.12"ID</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#9056k76/=19bq239</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#8974k16/=19bq4f4</t>
+  </si>
+  <si>
+    <t>aluminum rod 1.25"OD</t>
+  </si>
+  <si>
+    <t>20 guage</t>
+  </si>
+  <si>
+    <t>https://www.etsy.com/listing/62082177/copper-discs-20-gauge-stamping-blanks</t>
+  </si>
+  <si>
+    <t>Electrical Connects</t>
+  </si>
+  <si>
+    <t>copper disk 3/4"</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B003HGHQVU/ref=biss_dp_t_asn</t>
+  </si>
+  <si>
+    <t>copper braid</t>
+  </si>
+  <si>
+    <t>roll</t>
+  </si>
+  <si>
+    <t>25'x.25"</t>
+  </si>
+  <si>
+    <t>compression spring</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#9657k314/=19bqcva</t>
+  </si>
+  <si>
+    <t>1"Long .49"ID</t>
+  </si>
+  <si>
+    <t>Ring Terminal</t>
+  </si>
+  <si>
+    <t>.25"IDx.49"OD</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#7113k444/=19bqfh1</t>
+  </si>
+  <si>
+    <t>Copper Terminal screw .25"</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#92949a832/=19bqg8g</t>
+  </si>
+  <si>
+    <t>1/4"-20, 1/4"length</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#91251a146/=19bqn03</t>
+  </si>
+  <si>
+    <t>Black Oxide Screw .375"</t>
   </si>
 </sst>
 </file>
@@ -475,7 +547,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,7 +668,7 @@
         <v>33</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L7" si="0">E3*F3*I3*(1+J3)</f>
+        <f t="shared" ref="L3:L15" si="0">E3*F3*I3*(1+J3)</f>
         <v>7.3548000000000009</v>
       </c>
       <c r="M3">
@@ -640,7 +712,7 @@
         <v>8.1648000000000014</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M7" si="1">M3+L4</f>
+        <f t="shared" ref="M4:M15" si="1">M3+L4</f>
         <v>66.549599999999998</v>
       </c>
     </row>
@@ -727,7 +799,27 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D7" s="2"/>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>12.1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
       <c r="I7">
         <v>1</v>
       </c>
@@ -739,27 +831,310 @@
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13.068</v>
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>117.18</v>
+        <v>130.24800000000002</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D8" s="2"/>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>11.04</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0.08</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>11.9232</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>142.17120000000003</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D9" s="2"/>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9">
+        <f>10.35/12</f>
+        <v>0.86249999999999993</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0.08</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>11.178000000000001</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>153.34920000000002</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D10" s="2"/>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10">
+        <f>8.42/100</f>
+        <v>8.4199999999999997E-2</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0.08</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10" si="2">E10*F10*I10*(1+J10)</f>
+        <v>9.0936000000000003</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10" si="3">M9+L10</f>
+        <v>162.44280000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>162.44280000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <f>4/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="F12">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0.08</v>
+      </c>
+      <c r="K12">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>30.240000000000002</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>192.68280000000004</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D13" s="2"/>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0.08</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>21.610800000000005</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>214.29360000000005</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D14" s="2"/>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14">
+        <f>12.92/25</f>
+        <v>0.51680000000000004</v>
+      </c>
+      <c r="F14">
+        <v>25</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0.08</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>13.953600000000003</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>228.24720000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15">
+        <f>7.03/50</f>
+        <v>0.1406</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0.08</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>7.5924000000000005</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>235.83960000000005</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D16" s="2"/>
@@ -806,8 +1181,15 @@
     <hyperlink ref="D4" r:id="rId3" location="9008k78/=19bno32" xr:uid="{3E248846-5CE3-470E-A5E7-5ED38B41D492}"/>
     <hyperlink ref="D5" r:id="rId4" location="91251a158/=19bnq2t" xr:uid="{6CF9EFF7-6077-47C6-B406-2905E3FA64D1}"/>
     <hyperlink ref="D6" r:id="rId5" location="8585k205/=19bof2z" xr:uid="{04AB373F-6377-4008-A03D-91B129D7D564}"/>
+    <hyperlink ref="D7" r:id="rId6" location="9056k76/=19bq239" xr:uid="{6163FAE3-45EA-4697-A0DA-8C1CB1778A7D}"/>
+    <hyperlink ref="D8" r:id="rId7" location="8974k16/=19bq4f4" xr:uid="{A0ECCCBA-A525-462F-8F89-0C0F85CC72BC}"/>
+    <hyperlink ref="D12" r:id="rId8" xr:uid="{B38CFB83-B956-423D-8EA1-75263D11055F}"/>
+    <hyperlink ref="D9" r:id="rId9" location="9657k314/=19bqcva" xr:uid="{7DE85923-375E-48B5-92A8-92802E127ED3}"/>
+    <hyperlink ref="D14" r:id="rId10" location="7113k444/=19bqfh1" xr:uid="{102534B3-9837-4416-B56B-ADE837D3F460}"/>
+    <hyperlink ref="D15" r:id="rId11" location="92949a832/=19bqg8g" xr:uid="{819A1A06-5A78-4EB7-AB2C-84C8C8F90327}"/>
+    <hyperlink ref="D10" r:id="rId12" location="91251a146/=19bqn03" xr:uid="{26F3856E-872D-449F-BA72-95EFD8CA515B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CNC cam file start, BOM update
</commit_message>
<xml_diff>
--- a/BOM/BatteryHolder/BatHolder.xlsx
+++ b/BOM/BatteryHolder/BatHolder.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>Item Name</t>
   </si>
@@ -177,6 +177,54 @@
   </si>
   <si>
     <t>Black Oxide Screw .375"</t>
+  </si>
+  <si>
+    <t>EndMill .125"</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#2802a83/=19br6rt</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>2 ended, .75" cut length</t>
+  </si>
+  <si>
+    <t>Tooling</t>
+  </si>
+  <si>
+    <t>Purchase Total</t>
+  </si>
+  <si>
+    <t>Copper Bar</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#8966k15/=19brdi6</t>
+  </si>
+  <si>
+    <t>inches</t>
+  </si>
+  <si>
+    <t>1.125"OD</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Remington-Industries-18SNSP-Enameled-Diameter/dp/B00BJMVK02/ref=sr_1_1?ie=UTF8&amp;qid=1505074082&amp;sr=8-1&amp;keywords=18+gauge+magnet+wire</t>
+  </si>
+  <si>
+    <t>Magnet wire 18 AWG</t>
+  </si>
+  <si>
+    <t>18AWG</t>
+  </si>
+  <si>
+    <t>drill bit</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#2901a116/=19brqzs</t>
+  </si>
+  <si>
+    <t>9/64" 1.53" cut depth</t>
   </si>
 </sst>
 </file>
@@ -544,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00748F7B-54B9-4908-9896-05F30F59DACC}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,9 +607,10 @@
     <col min="8" max="8" width="24.6640625" customWidth="1"/>
     <col min="12" max="12" width="8.33203125" customWidth="1"/>
     <col min="13" max="13" width="11.21875" customWidth="1"/>
+    <col min="14" max="14" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -598,8 +647,11 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>15</v>
@@ -634,11 +686,15 @@
         <v>51.03</v>
       </c>
       <c r="M2">
-        <f>L2+K2</f>
+        <f>K2+L2</f>
         <v>51.03</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2">
+        <f>IF(C2="Y",0,L2+K2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -668,504 +724,745 @@
         <v>33</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L15" si="0">E3*F3*I3*(1+J3)</f>
+        <f>E3*F3*I3*(1+J3)</f>
         <v>7.3548000000000009</v>
       </c>
       <c r="M3">
-        <f>M2+L3</f>
-        <v>58.384799999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+        <f>K3+L3+M2</f>
+        <v>91.384799999999998</v>
+      </c>
+      <c r="N3">
+        <f>IF(C3="Y",0,L3+K3+N2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F4">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0.08</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="0"/>
-        <v>8.1648000000000014</v>
-      </c>
-      <c r="M4">
-        <f t="shared" ref="M4:M15" si="1">M3+L4</f>
-        <v>66.549599999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F5">
+        <f>5*9+10</f>
+        <v>55</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.08</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L18" si="0">E5*F5*I5*(1+J5)</f>
+        <v>16.632000000000005</v>
+      </c>
+      <c r="M5">
+        <f>K5+L5+M3</f>
+        <v>108.0168</v>
+      </c>
+      <c r="N5">
+        <f>IF(C5="Y",0,L5+K5+N3)</f>
+        <v>16.632000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <f>7.1/50</f>
         <v>0.14199999999999999</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>50</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" t="s">
         <v>20</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0.08</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0.08</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="0"/>
         <v>7.6680000000000001</v>
       </c>
-      <c r="M5">
-        <f t="shared" si="1"/>
-        <v>74.217600000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="M6">
+        <f>K6+L6+M5</f>
+        <v>115.68480000000001</v>
+      </c>
+      <c r="N6">
+        <f>IF(C6="Y",0,L6+K6+N5)</f>
+        <v>24.300000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E7" s="3">
         <f>19.89/8</f>
         <v>2.4862500000000001</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>16</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>26</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0.08</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0.08</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="0"/>
         <v>42.962400000000002</v>
       </c>
-      <c r="M6">
-        <f t="shared" si="1"/>
-        <v>117.18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="M7">
+        <f>K7+L7+M6</f>
+        <v>158.6472</v>
+      </c>
+      <c r="N7">
+        <f>IF(C7="Y",0,L7+K7+N6)</f>
+        <v>67.262400000000014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>12.1</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>28</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0.08</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0.08</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="0"/>
         <v>13.068</v>
       </c>
-      <c r="M7">
-        <f t="shared" si="1"/>
-        <v>130.24800000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="M8">
+        <f>K8+L8+M7</f>
+        <v>171.71520000000001</v>
+      </c>
+      <c r="N8">
+        <f>IF(C8="Y",0,L8+K8+N7)</f>
+        <v>80.330400000000012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>11.04</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0.08</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0.08</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="0"/>
         <v>11.9232</v>
       </c>
-      <c r="M8">
-        <f t="shared" si="1"/>
-        <v>142.17120000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="M9">
+        <f>K9+L9+M8</f>
+        <v>183.63840000000002</v>
+      </c>
+      <c r="N9">
+        <f>IF(C9="Y",0,L9+K9+N8)</f>
+        <v>92.253600000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <f>10.35/12</f>
         <v>0.86249999999999993</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>12</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>19</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>42</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0.08</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0.08</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="0"/>
         <v>11.178000000000001</v>
       </c>
-      <c r="M9">
-        <f t="shared" si="1"/>
-        <v>153.34920000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="M10">
+        <f>K10+L10+M9</f>
+        <v>194.81640000000002</v>
+      </c>
+      <c r="N10">
+        <f>IF(C10="Y",0,L10+K10+N9)</f>
+        <v>103.4316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>50</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <f>8.42/100</f>
         <v>8.4199999999999997E-2</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>100</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>19</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>20</v>
       </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>0.08</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <f t="shared" ref="L10" si="2">E10*F10*I10*(1+J10)</f>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0.08</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11" si="1">E11*F11*I11*(1+J11)</f>
         <v>9.0936000000000003</v>
       </c>
-      <c r="M10">
-        <f t="shared" ref="M10" si="3">M9+L10</f>
-        <v>162.44280000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="M11">
+        <f>K11+L11+M10</f>
+        <v>203.91000000000003</v>
+      </c>
+      <c r="N11">
+        <f>IF(C11="Y",0,L11+K11+N10)</f>
+        <v>112.5252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="L11">
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11">
-        <f t="shared" si="1"/>
-        <v>162.44280000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="M12">
+        <f>K12+L12+M11</f>
+        <v>203.91000000000003</v>
+      </c>
+      <c r="N12">
+        <f>IF(C12="Y",0,L12+K12+N11)</f>
+        <v>112.5252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <f>4/10</f>
         <v>0.4</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>70</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>19</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>32</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>0.08</v>
-      </c>
-      <c r="K12">
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0.08</v>
+      </c>
+      <c r="K13">
         <v>4.5999999999999996</v>
       </c>
-      <c r="L12">
+      <c r="L13">
         <f t="shared" si="0"/>
         <v>30.240000000000002</v>
       </c>
-      <c r="M12">
-        <f t="shared" si="1"/>
-        <v>192.68280000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="M13">
+        <f>K13+L13+M12</f>
+        <v>238.75000000000003</v>
+      </c>
+      <c r="N13">
+        <f>IF(C13="Y",0,L13+K13+N12)</f>
+        <v>147.36520000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>20.010000000000002</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
         <v>38</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
         <v>39</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>0.08</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0.08</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="0"/>
         <v>21.610800000000005</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="1"/>
-        <v>214.29360000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="M14">
+        <f>K14+L14+M13</f>
+        <v>260.36080000000004</v>
+      </c>
+      <c r="N14">
+        <f>IF(C14="Y",0,L14+K14+N13)</f>
+        <v>168.97600000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>43</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <f>12.92/25</f>
         <v>0.51680000000000004</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>25</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>19</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H15" t="s">
         <v>44</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>0.08</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0.08</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="0"/>
         <v>13.953600000000003</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="1"/>
-        <v>228.24720000000005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="M15">
+        <f>K15+L15+M14</f>
+        <v>274.31440000000003</v>
+      </c>
+      <c r="N15">
+        <f>IF(C15="Y",0,L15+K15+N14)</f>
+        <v>182.92960000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <f>7.03/50</f>
         <v>0.1406</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>50</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>19</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H16" t="s">
         <v>48</v>
       </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>0.08</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0.08</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="0"/>
         <v>7.5924000000000005</v>
       </c>
-      <c r="M15">
-        <f t="shared" si="1"/>
-        <v>235.83960000000005</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D16" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <f>K16+L16+M15</f>
+        <v>281.90680000000003</v>
+      </c>
+      <c r="N16">
+        <f>IF(C16="Y",0,L16+K16+N15)</f>
+        <v>190.52200000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17">
+        <f>39.58/6</f>
+        <v>6.5966666666666667</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0.08</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>42.746400000000001</v>
+      </c>
+      <c r="M17">
+        <f>K17+L17+M16</f>
+        <v>324.65320000000003</v>
+      </c>
+      <c r="N17">
+        <f>IF(C17="Y",0,L17+K17+N16)</f>
+        <v>233.26840000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18">
+        <f>16.73/201</f>
+        <v>8.3233830845771142E-2</v>
+      </c>
+      <c r="F18">
+        <v>201</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0.08</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>18.0684</v>
+      </c>
+      <c r="M18">
+        <f>K18+L18+M17</f>
+        <v>342.72160000000002</v>
+      </c>
+      <c r="N18">
+        <f>IF(C18="Y",0,L18+K18+N17)</f>
+        <v>251.33680000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="M19">
+        <f>K19+L19+M18</f>
+        <v>342.72160000000002</v>
+      </c>
+      <c r="N19">
+        <f>IF(C19="Y",0,L19+K19+N18)</f>
+        <v>251.33680000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20">
+        <v>23.65</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0.08</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f>E20*F20*I20*(1+J20)</f>
+        <v>25.542000000000002</v>
+      </c>
+      <c r="M20">
+        <f>K20+L20+M19</f>
+        <v>368.2636</v>
+      </c>
+      <c r="N20">
+        <f>IF(C20="Y",0,L20+K20+N19)</f>
+        <v>276.87880000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21">
+        <v>1.67</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" t="s">
+        <v>66</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0.08</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f>E21*F21*I21*(1+J21)</f>
+        <v>7.2144000000000004</v>
+      </c>
+      <c r="M21">
+        <f>K21+L21+M20</f>
+        <v>375.47800000000001</v>
+      </c>
+      <c r="N21">
+        <f>IF(C21="Y",0,L21+K21+N20)</f>
+        <v>284.09320000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D30" s="2"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.3">
@@ -1178,18 +1475,22 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" location="8975k617/=19bnny9" xr:uid="{18A7086B-4922-4F21-A85F-453934409742}"/>
     <hyperlink ref="D3" r:id="rId2" location="9008k78/=19bno32" xr:uid="{0903AB3E-4941-460C-8B26-6317F3CB18E0}"/>
-    <hyperlink ref="D4" r:id="rId3" location="9008k78/=19bno32" xr:uid="{3E248846-5CE3-470E-A5E7-5ED38B41D492}"/>
-    <hyperlink ref="D5" r:id="rId4" location="91251a158/=19bnq2t" xr:uid="{6CF9EFF7-6077-47C6-B406-2905E3FA64D1}"/>
-    <hyperlink ref="D6" r:id="rId5" location="8585k205/=19bof2z" xr:uid="{04AB373F-6377-4008-A03D-91B129D7D564}"/>
-    <hyperlink ref="D7" r:id="rId6" location="9056k76/=19bq239" xr:uid="{6163FAE3-45EA-4697-A0DA-8C1CB1778A7D}"/>
-    <hyperlink ref="D8" r:id="rId7" location="8974k16/=19bq4f4" xr:uid="{A0ECCCBA-A525-462F-8F89-0C0F85CC72BC}"/>
-    <hyperlink ref="D12" r:id="rId8" xr:uid="{B38CFB83-B956-423D-8EA1-75263D11055F}"/>
-    <hyperlink ref="D9" r:id="rId9" location="9657k314/=19bqcva" xr:uid="{7DE85923-375E-48B5-92A8-92802E127ED3}"/>
-    <hyperlink ref="D14" r:id="rId10" location="7113k444/=19bqfh1" xr:uid="{102534B3-9837-4416-B56B-ADE837D3F460}"/>
-    <hyperlink ref="D15" r:id="rId11" location="92949a832/=19bqg8g" xr:uid="{819A1A06-5A78-4EB7-AB2C-84C8C8F90327}"/>
-    <hyperlink ref="D10" r:id="rId12" location="91251a146/=19bqn03" xr:uid="{26F3856E-872D-449F-BA72-95EFD8CA515B}"/>
+    <hyperlink ref="D5" r:id="rId3" location="9008k78/=19bno32" xr:uid="{3E248846-5CE3-470E-A5E7-5ED38B41D492}"/>
+    <hyperlink ref="D6" r:id="rId4" location="91251a158/=19bnq2t" xr:uid="{6CF9EFF7-6077-47C6-B406-2905E3FA64D1}"/>
+    <hyperlink ref="D7" r:id="rId5" location="8585k205/=19bof2z" xr:uid="{04AB373F-6377-4008-A03D-91B129D7D564}"/>
+    <hyperlink ref="D8" r:id="rId6" location="9056k76/=19bq239" xr:uid="{6163FAE3-45EA-4697-A0DA-8C1CB1778A7D}"/>
+    <hyperlink ref="D9" r:id="rId7" location="8974k16/=19bq4f4" xr:uid="{A0ECCCBA-A525-462F-8F89-0C0F85CC72BC}"/>
+    <hyperlink ref="D13" r:id="rId8" xr:uid="{B38CFB83-B956-423D-8EA1-75263D11055F}"/>
+    <hyperlink ref="D10" r:id="rId9" location="9657k314/=19bqcva" xr:uid="{7DE85923-375E-48B5-92A8-92802E127ED3}"/>
+    <hyperlink ref="D15" r:id="rId10" location="7113k444/=19bqfh1" xr:uid="{102534B3-9837-4416-B56B-ADE837D3F460}"/>
+    <hyperlink ref="D16" r:id="rId11" location="92949a832/=19bqg8g" xr:uid="{819A1A06-5A78-4EB7-AB2C-84C8C8F90327}"/>
+    <hyperlink ref="D11" r:id="rId12" location="91251a146/=19bqn03" xr:uid="{26F3856E-872D-449F-BA72-95EFD8CA515B}"/>
+    <hyperlink ref="D20" r:id="rId13" location="2802a83/=19br6rt" xr:uid="{2B71B782-19F3-40B2-8B57-4BCD705D8E1D}"/>
+    <hyperlink ref="D17" r:id="rId14" location="8966k15/=19brdi6" xr:uid="{FE8BB7CF-EB44-44F3-A161-F736592B276A}"/>
+    <hyperlink ref="D18" r:id="rId15" xr:uid="{54C62218-F532-41FA-B7D5-86FB16B75781}"/>
+    <hyperlink ref="D21" r:id="rId16" location="2901a116/=19brqzs" xr:uid="{2009869C-D1B6-4696-A13F-91F4FFFEFA2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
grind rails and updated bat holder assembly
</commit_message>
<xml_diff>
--- a/BOM/BatteryHolder/BatHolder.xlsx
+++ b/BOM/BatteryHolder/BatHolder.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>Item Name</t>
   </si>
@@ -89,15 +89,9 @@
     <t>6-32 thread</t>
   </si>
   <si>
-    <t>Black Oxide Screw 1.75"</t>
-  </si>
-  <si>
     <t>Aluminum spacers 5/16"</t>
   </si>
   <si>
-    <t>https://www.mcmaster.com/#91251a158/=19bnq2t</t>
-  </si>
-  <si>
     <t>https://www.mcmaster.com/#8585k205/=19bof2z</t>
   </si>
   <si>
@@ -225,6 +219,18 @@
   </si>
   <si>
     <t>9/64" 1.53" cut depth</t>
+  </si>
+  <si>
+    <t>Black Oxide Screw 1.50"</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#91251a157/=19evjrx</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#8975k91/=19evlb8</t>
+  </si>
+  <si>
+    <t>6'x3 1/2"x3/8" Aluminum</t>
   </si>
 </sst>
 </file>
@@ -251,12 +257,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,11 +290,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -592,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00748F7B-54B9-4908-9896-05F30F59DACC}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,7 +630,7 @@
     <col min="14" max="14" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -648,13 +668,13 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -694,7 +714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -732,16 +752,59 @@
         <v>91.384799999999998</v>
       </c>
       <c r="N3">
-        <f>IF(C3="Y",0,L3+K3+N2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <f t="shared" ref="N3:N14" si="0">IF(C3="Y",N2,L3+K3+N2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4">
+        <f>18.77/2</f>
+        <v>9.3849999999999998</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.08</v>
+      </c>
+      <c r="K4">
+        <v>33</v>
+      </c>
+      <c r="L4">
+        <f>E4*F4*I4*(1+J4)</f>
+        <v>20.271599999999999</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M21" si="1">K4+L4+M3</f>
+        <v>144.65639999999999</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>17</v>
@@ -769,31 +832,31 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L18" si="0">E5*F5*I5*(1+J5)</f>
+        <f t="shared" ref="L5:L18" si="2">E5*F5*I5*(1+J5)</f>
         <v>16.632000000000005</v>
       </c>
       <c r="M5">
-        <f>K5+L5+M3</f>
-        <v>108.0168</v>
+        <f t="shared" si="1"/>
+        <v>161.2884</v>
       </c>
       <c r="N5">
-        <f>IF(C5="Y",0,L5+K5+N3)</f>
-        <v>16.632000000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="E6">
-        <f>7.1/50</f>
-        <v>0.14199999999999999</v>
+        <f>9.94/50</f>
+        <v>0.19879999999999998</v>
       </c>
       <c r="F6">
         <v>50</v>
@@ -814,27 +877,27 @@
         <v>0</v>
       </c>
       <c r="L6">
+        <f t="shared" si="2"/>
+        <v>10.735200000000001</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>172.02359999999999</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="0"/>
-        <v>7.6680000000000001</v>
-      </c>
-      <c r="M6">
-        <f>K6+L6+M5</f>
-        <v>115.68480000000001</v>
-      </c>
-      <c r="N6">
-        <f>IF(C6="Y",0,L6+K6+N5)</f>
-        <v>24.300000000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3">
         <f>19.89/8</f>
@@ -847,7 +910,7 @@
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -859,27 +922,27 @@
         <v>0</v>
       </c>
       <c r="L7">
+        <f t="shared" si="2"/>
+        <v>42.962400000000002</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>214.98599999999999</v>
+      </c>
+      <c r="N7">
         <f t="shared" si="0"/>
-        <v>42.962400000000002</v>
-      </c>
-      <c r="M7">
-        <f>K7+L7+M6</f>
-        <v>158.6472</v>
-      </c>
-      <c r="N7">
-        <f>IF(C7="Y",0,L7+K7+N6)</f>
-        <v>67.262400000000014</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="E8">
         <v>12.1</v>
@@ -891,45 +954,46 @@
         <v>18</v>
       </c>
       <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0.08</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>13.068</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>228.054</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0.08</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>13.068</v>
-      </c>
-      <c r="M8">
-        <f>K8+L8+M7</f>
-        <v>171.71520000000001</v>
-      </c>
-      <c r="N8">
-        <f>IF(C8="Y",0,L8+K8+N7)</f>
-        <v>80.330400000000012</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="E9">
-        <v>11.04</v>
+        <f>21.08/2</f>
+        <v>10.54</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
@@ -944,27 +1008,27 @@
         <v>0</v>
       </c>
       <c r="L9">
+        <f t="shared" si="2"/>
+        <v>22.766400000000001</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>250.82040000000001</v>
+      </c>
+      <c r="N9">
         <f t="shared" si="0"/>
-        <v>11.9232</v>
-      </c>
-      <c r="M9">
-        <f>K9+L9+M8</f>
-        <v>183.63840000000002</v>
-      </c>
-      <c r="N9">
-        <f>IF(C9="Y",0,L9+K9+N8)</f>
-        <v>92.253600000000006</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10">
         <f>10.35/12</f>
@@ -977,7 +1041,7 @@
         <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -989,27 +1053,27 @@
         <v>0</v>
       </c>
       <c r="L10">
+        <f t="shared" si="2"/>
+        <v>11.178000000000001</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>261.9984</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="0"/>
-        <v>11.178000000000001</v>
-      </c>
-      <c r="M10">
-        <f>K10+L10+M9</f>
-        <v>194.81640000000002</v>
-      </c>
-      <c r="N10">
-        <f>IF(C10="Y",0,L10+K10+N9)</f>
-        <v>103.4316</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11">
         <f>8.42/100</f>
@@ -1034,60 +1098,60 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11" si="1">E11*F11*I11*(1+J11)</f>
+        <f t="shared" ref="L11" si="3">E11*F11*I11*(1+J11)</f>
         <v>9.0936000000000003</v>
       </c>
       <c r="M11">
-        <f>K11+L11+M10</f>
-        <v>203.91000000000003</v>
+        <f t="shared" si="1"/>
+        <v>271.09199999999998</v>
       </c>
       <c r="N11">
-        <f>IF(C11="Y",0,L11+K11+N10)</f>
-        <v>112.5252</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="L12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>271.09199999999998</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M12">
-        <f>K12+L12+M11</f>
-        <v>203.91000000000003</v>
-      </c>
-      <c r="N12">
-        <f>IF(C12="Y",0,L12+K12+N11)</f>
-        <v>112.5252</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E13">
         <f>4/10</f>
         <v>0.4</v>
       </c>
       <c r="F13">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1096,30 +1160,30 @@
         <v>0.08</v>
       </c>
       <c r="K13">
-        <v>4.5999999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="L13">
+        <f t="shared" si="2"/>
+        <v>34.56</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>310.35199999999998</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="0"/>
-        <v>30.240000000000002</v>
-      </c>
-      <c r="M13">
-        <f>K13+L13+M12</f>
-        <v>238.75000000000003</v>
-      </c>
-      <c r="N13">
-        <f>IF(C13="Y",0,L13+K13+N12)</f>
-        <v>147.36520000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14">
         <v>20.010000000000002</v>
@@ -1128,10 +1192,10 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1143,27 +1207,27 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>21.610800000000005</v>
       </c>
       <c r="M14">
         <f>K14+L14+M13</f>
-        <v>260.36080000000004</v>
+        <v>331.96279999999996</v>
       </c>
       <c r="N14">
-        <f>IF(C14="Y",0,L14+K14+N13)</f>
-        <v>168.97600000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="E15">
         <f>12.92/25</f>
@@ -1176,39 +1240,39 @@
         <v>19</v>
       </c>
       <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0.08</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>13.953600000000003</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>345.91639999999995</v>
+      </c>
+      <c r="N15">
+        <f>IF(C15="Y",N14,L15+K15+N14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>0.08</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="0"/>
-        <v>13.953600000000003</v>
-      </c>
-      <c r="M15">
-        <f>K15+L15+M14</f>
-        <v>274.31440000000003</v>
-      </c>
-      <c r="N15">
-        <f>IF(C15="Y",0,L15+K15+N14)</f>
-        <v>182.92960000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E16">
         <f>7.03/50</f>
@@ -1221,7 +1285,7 @@
         <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1233,40 +1297,41 @@
         <v>0</v>
       </c>
       <c r="L16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.5924000000000005</v>
       </c>
       <c r="M16">
-        <f>K16+L16+M15</f>
-        <v>281.90680000000003</v>
+        <f t="shared" si="1"/>
+        <v>353.50879999999995</v>
       </c>
       <c r="N16">
-        <f>IF(C16="Y",0,L16+K16+N15)</f>
-        <v>190.52200000000002</v>
+        <f t="shared" ref="N16:N21" si="4">IF(C16="Y",N15,L16+K16+N15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E17">
         <f>39.58/6</f>
         <v>6.5966666666666667</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -1278,27 +1343,27 @@
         <v>0</v>
       </c>
       <c r="L17">
-        <f t="shared" si="0"/>
-        <v>42.746400000000001</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="M17">
-        <f>K17+L17+M16</f>
-        <v>324.65320000000003</v>
+        <f t="shared" si="1"/>
+        <v>353.50879999999995</v>
       </c>
       <c r="N17">
-        <f>IF(C17="Y",0,L17+K17+N16)</f>
-        <v>233.26840000000001</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18">
         <f>16.73/201</f>
@@ -1311,7 +1376,7 @@
         <v>18</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -1323,52 +1388,53 @@
         <v>0</v>
       </c>
       <c r="L18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>18.0684</v>
       </c>
       <c r="M18">
-        <f>K18+L18+M17</f>
-        <v>342.72160000000002</v>
+        <f t="shared" si="1"/>
+        <v>371.57719999999995</v>
       </c>
       <c r="N18">
-        <f>IF(C18="Y",0,L18+K18+N17)</f>
-        <v>251.33680000000001</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M19">
-        <f>K19+L19+M18</f>
-        <v>342.72160000000002</v>
+        <f t="shared" si="1"/>
+        <v>371.57719999999995</v>
       </c>
       <c r="N19">
-        <f>IF(C19="Y",0,L19+K19+N18)</f>
-        <v>251.33680000000001</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E20">
         <v>23.65</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -1381,26 +1447,26 @@
       </c>
       <c r="L20">
         <f>E20*F20*I20*(1+J20)</f>
-        <v>25.542000000000002</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <f>K20+L20+M19</f>
-        <v>368.2636</v>
+        <f t="shared" si="1"/>
+        <v>371.57719999999995</v>
       </c>
       <c r="N20">
-        <f>IF(C20="Y",0,L20+K20+N19)</f>
-        <v>276.87880000000001</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E21">
         <v>1.67</v>
@@ -1409,10 +1475,10 @@
         <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -1428,16 +1494,15 @@
         <v>7.2144000000000004</v>
       </c>
       <c r="M21">
-        <f>K21+L21+M20</f>
-        <v>375.47800000000001</v>
+        <f t="shared" si="1"/>
+        <v>378.79159999999996</v>
       </c>
       <c r="N21">
-        <f>IF(C21="Y",0,L21+K21+N20)</f>
-        <v>284.09320000000002</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="D22" s="2"/>
     </row>
@@ -1476,21 +1541,23 @@
     <hyperlink ref="D2" r:id="rId1" location="8975k617/=19bnny9" xr:uid="{18A7086B-4922-4F21-A85F-453934409742}"/>
     <hyperlink ref="D3" r:id="rId2" location="9008k78/=19bno32" xr:uid="{0903AB3E-4941-460C-8B26-6317F3CB18E0}"/>
     <hyperlink ref="D5" r:id="rId3" location="9008k78/=19bno32" xr:uid="{3E248846-5CE3-470E-A5E7-5ED38B41D492}"/>
-    <hyperlink ref="D6" r:id="rId4" location="91251a158/=19bnq2t" xr:uid="{6CF9EFF7-6077-47C6-B406-2905E3FA64D1}"/>
-    <hyperlink ref="D7" r:id="rId5" location="8585k205/=19bof2z" xr:uid="{04AB373F-6377-4008-A03D-91B129D7D564}"/>
-    <hyperlink ref="D8" r:id="rId6" location="9056k76/=19bq239" xr:uid="{6163FAE3-45EA-4697-A0DA-8C1CB1778A7D}"/>
-    <hyperlink ref="D9" r:id="rId7" location="8974k16/=19bq4f4" xr:uid="{A0ECCCBA-A525-462F-8F89-0C0F85CC72BC}"/>
-    <hyperlink ref="D13" r:id="rId8" xr:uid="{B38CFB83-B956-423D-8EA1-75263D11055F}"/>
-    <hyperlink ref="D10" r:id="rId9" location="9657k314/=19bqcva" xr:uid="{7DE85923-375E-48B5-92A8-92802E127ED3}"/>
-    <hyperlink ref="D15" r:id="rId10" location="7113k444/=19bqfh1" xr:uid="{102534B3-9837-4416-B56B-ADE837D3F460}"/>
-    <hyperlink ref="D16" r:id="rId11" location="92949a832/=19bqg8g" xr:uid="{819A1A06-5A78-4EB7-AB2C-84C8C8F90327}"/>
-    <hyperlink ref="D11" r:id="rId12" location="91251a146/=19bqn03" xr:uid="{26F3856E-872D-449F-BA72-95EFD8CA515B}"/>
-    <hyperlink ref="D20" r:id="rId13" location="2802a83/=19br6rt" xr:uid="{2B71B782-19F3-40B2-8B57-4BCD705D8E1D}"/>
-    <hyperlink ref="D17" r:id="rId14" location="8966k15/=19brdi6" xr:uid="{FE8BB7CF-EB44-44F3-A161-F736592B276A}"/>
-    <hyperlink ref="D18" r:id="rId15" xr:uid="{54C62218-F532-41FA-B7D5-86FB16B75781}"/>
-    <hyperlink ref="D21" r:id="rId16" location="2901a116/=19brqzs" xr:uid="{2009869C-D1B6-4696-A13F-91F4FFFEFA2F}"/>
+    <hyperlink ref="D7" r:id="rId4" location="8585k205/=19bof2z" xr:uid="{04AB373F-6377-4008-A03D-91B129D7D564}"/>
+    <hyperlink ref="D8" r:id="rId5" location="9056k76/=19bq239" xr:uid="{6163FAE3-45EA-4697-A0DA-8C1CB1778A7D}"/>
+    <hyperlink ref="D9" r:id="rId6" location="8974k16/=19bq4f4" xr:uid="{A0ECCCBA-A525-462F-8F89-0C0F85CC72BC}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{B38CFB83-B956-423D-8EA1-75263D11055F}"/>
+    <hyperlink ref="D10" r:id="rId8" location="9657k314/=19bqcva" xr:uid="{7DE85923-375E-48B5-92A8-92802E127ED3}"/>
+    <hyperlink ref="D15" r:id="rId9" location="7113k444/=19bqfh1" xr:uid="{102534B3-9837-4416-B56B-ADE837D3F460}"/>
+    <hyperlink ref="D16" r:id="rId10" location="92949a832/=19bqg8g" xr:uid="{819A1A06-5A78-4EB7-AB2C-84C8C8F90327}"/>
+    <hyperlink ref="D11" r:id="rId11" location="91251a146/=19bqn03" xr:uid="{26F3856E-872D-449F-BA72-95EFD8CA515B}"/>
+    <hyperlink ref="D20" r:id="rId12" location="2802a83/=19br6rt" xr:uid="{2B71B782-19F3-40B2-8B57-4BCD705D8E1D}"/>
+    <hyperlink ref="D17" r:id="rId13" location="8966k15/=19brdi6" xr:uid="{FE8BB7CF-EB44-44F3-A161-F736592B276A}"/>
+    <hyperlink ref="D18" r:id="rId14" xr:uid="{54C62218-F532-41FA-B7D5-86FB16B75781}"/>
+    <hyperlink ref="D21" r:id="rId15" location="2901a116/=19brqzs" xr:uid="{2009869C-D1B6-4696-A13F-91F4FFFEFA2F}"/>
+    <hyperlink ref="D6" r:id="rId16" location="91251a157/=19evjrx" xr:uid="{7C801063-5A3E-4AAE-8536-CB3E6CF8B1F7}"/>
+    <hyperlink ref="D4" r:id="rId17" location="8975k91/=19evlb8" xr:uid="{3EED6DB3-513A-4A9B-A132-2DF3D8EB3CFF}"/>
+    <hyperlink ref="D14" r:id="rId18" xr:uid="{1A45FFED-84A3-4DF1-94D9-66F1B415517E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mold update and redo
</commit_message>
<xml_diff>
--- a/BOM/BatteryHolder/BatHolder.xlsx
+++ b/BOM/BatteryHolder/BatHolder.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LongboardMarkII\BOM\BatteryHolder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danny Andreev\Documents\MarkII\LongboardMarkII\BOM\BatteryHolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="84">
   <si>
     <t>Item Name</t>
   </si>
@@ -231,6 +231,51 @@
   </si>
   <si>
     <t>6'x3 1/2"x3/8" Aluminum</t>
+  </si>
+  <si>
+    <t>Mold Machining work</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>machining work on mold at architecture school</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#91251a158/=19n12mv</t>
+  </si>
+  <si>
+    <t>Black Oxide Screw 1.75"</t>
+  </si>
+  <si>
+    <t>UNITS</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#8873a232/=19n144r</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>1/2"-1/16" carbid ball endmills</t>
+  </si>
+  <si>
+    <t>Ball Endmill 3/4"</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#2866a84/=19n16ap</t>
+  </si>
+  <si>
+    <t>4" length of cut</t>
+  </si>
+  <si>
+    <t>drill bit 3/16"</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#87755a29/=19n185a</t>
+  </si>
+  <si>
+    <t>1.75" length of cut</t>
   </si>
 </sst>
 </file>
@@ -614,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00748F7B-54B9-4908-9896-05F30F59DACC}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,7 +797,7 @@
         <v>91.384799999999998</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N14" si="0">IF(C3="Y",N2,L3+K3+N2)</f>
+        <f t="shared" ref="N3:N27" si="0">IF(C3="Y",N2,L3+K3+N2)</f>
         <v>0</v>
       </c>
     </row>
@@ -790,7 +835,7 @@
         <v>20.271599999999999</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M21" si="1">K4+L4+M3</f>
+        <f t="shared" ref="M4:M27" si="1">K4+L4+M3</f>
         <v>144.65639999999999</v>
       </c>
       <c r="N4">
@@ -813,8 +858,8 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="F5">
-        <f>5*9+10</f>
-        <v>55</v>
+        <f>5*9+30</f>
+        <v>75</v>
       </c>
       <c r="G5" t="s">
         <v>19</v>
@@ -832,12 +877,12 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L18" si="2">E5*F5*I5*(1+J5)</f>
-        <v>16.632000000000005</v>
+        <f t="shared" ref="L5:L10" si="2">E5*F5*I5*(1+J5)</f>
+        <v>22.680000000000007</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>161.2884</v>
+        <v>167.3364</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
@@ -882,7 +927,7 @@
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>172.02359999999999</v>
+        <v>178.07159999999999</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
@@ -927,7 +972,7 @@
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>214.98599999999999</v>
+        <v>221.03399999999999</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
@@ -971,7 +1016,7 @@
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>228.054</v>
+        <v>234.102</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
@@ -1013,7 +1058,7 @@
       </c>
       <c r="M9">
         <f t="shared" si="1"/>
-        <v>250.82040000000001</v>
+        <v>256.86840000000001</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
@@ -1058,7 +1103,7 @@
       </c>
       <c r="M10">
         <f t="shared" si="1"/>
-        <v>261.9984</v>
+        <v>268.04640000000001</v>
       </c>
       <c r="N10">
         <f t="shared" si="0"/>
@@ -1098,12 +1143,12 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11" si="3">E11*F11*I11*(1+J11)</f>
+        <f t="shared" ref="L11:L12" si="3">E11*F11*I11*(1+J11)</f>
         <v>9.0936000000000003</v>
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>271.09199999999998</v>
+        <v>277.14</v>
       </c>
       <c r="N11">
         <f t="shared" si="0"/>
@@ -1111,330 +1156,327 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12">
+        <f>7.1/50</f>
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0.08</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>7.6680000000000001</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>284.80799999999999</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>284.80799999999999</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="1"/>
-        <v>271.09199999999998</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f>E14*F14*I14*(1+J14)</f>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>284.80799999999999</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <f>4/10</f>
         <v>0.4</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>80</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G15" t="s">
         <v>19</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H15" t="s">
         <v>30</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>0.08</v>
-      </c>
-      <c r="K13">
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0.08</v>
+      </c>
+      <c r="K15">
         <v>4.7</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="2"/>
+      <c r="L15">
+        <f>E15*F15*I15*(1+J15)</f>
         <v>34.56</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="1"/>
-        <v>310.35199999999998</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>324.06799999999998</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E14">
+      <c r="E16">
         <v>20.010000000000002</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>36</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H16" t="s">
         <v>37</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>0.08</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="2"/>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0.08</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>E16*F16*I16*(1+J16)</f>
         <v>21.610800000000005</v>
       </c>
-      <c r="M14">
-        <f>K14+L14+M13</f>
-        <v>331.96279999999996</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>345.67879999999997</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <f>12.92/25</f>
         <v>0.51680000000000004</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <v>25</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G17" t="s">
         <v>19</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H17" t="s">
         <v>42</v>
       </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>0.08</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="2"/>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0.08</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>E17*F17*I17*(1+J17)</f>
         <v>13.953600000000003</v>
       </c>
-      <c r="M15">
-        <f t="shared" si="1"/>
-        <v>345.91639999999995</v>
-      </c>
-      <c r="N15">
-        <f>IF(C15="Y",N14,L15+K15+N14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>359.63239999999996</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E16">
+      <c r="E18">
         <f>7.03/50</f>
         <v>0.1406</v>
       </c>
-      <c r="F16">
+      <c r="F18">
         <v>50</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G18" t="s">
         <v>19</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H18" t="s">
         <v>46</v>
       </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>0.08</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="2"/>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0.08</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>E18*F18*I18*(1+J18)</f>
         <v>7.5924000000000005</v>
       </c>
-      <c r="M16">
-        <f t="shared" si="1"/>
-        <v>353.50879999999995</v>
-      </c>
-      <c r="N16">
-        <f t="shared" ref="N16:N21" si="4">IF(C16="Y",N15,L16+K16+N15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" t="s">
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>367.22479999999996</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" t="s">
         <v>55</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E17">
+      <c r="E19">
         <f>39.58/6</f>
         <v>6.5966666666666667</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
         <v>57</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H19" t="s">
         <v>58</v>
       </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>0.08</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="1"/>
-        <v>353.50879999999995</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0.08</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>E19*F19*I19*(1+J19)</f>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>367.22479999999996</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>60</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E18">
+      <c r="E20">
         <f>16.73/201</f>
         <v>8.3233830845771142E-2</v>
       </c>
-      <c r="F18">
+      <c r="F20">
         <v>201</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G20" t="s">
         <v>18</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H20" t="s">
         <v>61</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18">
-        <v>0.08</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="2"/>
-        <v>18.0684</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="1"/>
-        <v>371.57719999999995</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="1"/>
-        <v>371.57719999999995</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20">
-        <v>23.65</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" t="s">
-        <v>51</v>
-      </c>
-      <c r="H20" t="s">
-        <v>52</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -1447,79 +1489,290 @@
       </c>
       <c r="L20">
         <f>E20*F20*I20*(1+J20)</f>
-        <v>0</v>
+        <v>18.0684</v>
       </c>
       <c r="M20">
         <f t="shared" si="1"/>
-        <v>371.57719999999995</v>
+        <v>385.29319999999996</v>
       </c>
       <c r="N20">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>385.29319999999996</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22">
+        <v>23.65</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0.08</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f>E22*F22*I22*(1+J22)</f>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>385.29319999999996</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23">
+        <v>1.67</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0.08</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f>E23*F23*I23*(1+J23)</f>
+        <v>7.2144000000000004</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>392.50759999999997</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24">
+        <v>218</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0.08</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ref="L24:L26" si="4">E24*F24*I24*(1+J24)</f>
+        <v>235.44000000000003</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>627.94759999999997</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>7.6680000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25">
+        <v>109.68</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>0.08</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" t="s">
+        <v>118.45440000000002</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>746.40200000000004</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>126.12240000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26">
+        <v>2.21</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0.08</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="4"/>
+        <v>7.1604000000000001</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>753.56240000000003</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>133.28280000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21">
-        <v>1.67</v>
-      </c>
-      <c r="F21">
-        <v>4</v>
-      </c>
-      <c r="G21" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>0.08</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <f>E21*F21*I21*(1+J21)</f>
-        <v>7.2144000000000004</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="1"/>
-        <v>378.79159999999996</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D27" s="2"/>
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1.5</v>
+      </c>
+      <c r="L27">
+        <f>E27*F27*I27*(1+J27)</f>
+        <v>60</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>815.06240000000003</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>133.28280000000004</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D28" s="2"/>
@@ -1544,20 +1797,23 @@
     <hyperlink ref="D7" r:id="rId4" location="8585k205/=19bof2z" xr:uid="{04AB373F-6377-4008-A03D-91B129D7D564}"/>
     <hyperlink ref="D8" r:id="rId5" location="9056k76/=19bq239" xr:uid="{6163FAE3-45EA-4697-A0DA-8C1CB1778A7D}"/>
     <hyperlink ref="D9" r:id="rId6" location="8974k16/=19bq4f4" xr:uid="{A0ECCCBA-A525-462F-8F89-0C0F85CC72BC}"/>
-    <hyperlink ref="D13" r:id="rId7" xr:uid="{B38CFB83-B956-423D-8EA1-75263D11055F}"/>
+    <hyperlink ref="D15" r:id="rId7" xr:uid="{B38CFB83-B956-423D-8EA1-75263D11055F}"/>
     <hyperlink ref="D10" r:id="rId8" location="9657k314/=19bqcva" xr:uid="{7DE85923-375E-48B5-92A8-92802E127ED3}"/>
-    <hyperlink ref="D15" r:id="rId9" location="7113k444/=19bqfh1" xr:uid="{102534B3-9837-4416-B56B-ADE837D3F460}"/>
-    <hyperlink ref="D16" r:id="rId10" location="92949a832/=19bqg8g" xr:uid="{819A1A06-5A78-4EB7-AB2C-84C8C8F90327}"/>
+    <hyperlink ref="D17" r:id="rId9" location="7113k444/=19bqfh1" xr:uid="{102534B3-9837-4416-B56B-ADE837D3F460}"/>
+    <hyperlink ref="D18" r:id="rId10" location="92949a832/=19bqg8g" xr:uid="{819A1A06-5A78-4EB7-AB2C-84C8C8F90327}"/>
     <hyperlink ref="D11" r:id="rId11" location="91251a146/=19bqn03" xr:uid="{26F3856E-872D-449F-BA72-95EFD8CA515B}"/>
-    <hyperlink ref="D20" r:id="rId12" location="2802a83/=19br6rt" xr:uid="{2B71B782-19F3-40B2-8B57-4BCD705D8E1D}"/>
-    <hyperlink ref="D17" r:id="rId13" location="8966k15/=19brdi6" xr:uid="{FE8BB7CF-EB44-44F3-A161-F736592B276A}"/>
-    <hyperlink ref="D18" r:id="rId14" xr:uid="{54C62218-F532-41FA-B7D5-86FB16B75781}"/>
-    <hyperlink ref="D21" r:id="rId15" location="2901a116/=19brqzs" xr:uid="{2009869C-D1B6-4696-A13F-91F4FFFEFA2F}"/>
+    <hyperlink ref="D22" r:id="rId12" location="2802a83/=19br6rt" xr:uid="{2B71B782-19F3-40B2-8B57-4BCD705D8E1D}"/>
+    <hyperlink ref="D19" r:id="rId13" location="8966k15/=19brdi6" xr:uid="{FE8BB7CF-EB44-44F3-A161-F736592B276A}"/>
+    <hyperlink ref="D20" r:id="rId14" xr:uid="{54C62218-F532-41FA-B7D5-86FB16B75781}"/>
+    <hyperlink ref="D23" r:id="rId15" location="2901a116/=19brqzs" xr:uid="{2009869C-D1B6-4696-A13F-91F4FFFEFA2F}"/>
     <hyperlink ref="D6" r:id="rId16" location="91251a157/=19evjrx" xr:uid="{7C801063-5A3E-4AAE-8536-CB3E6CF8B1F7}"/>
     <hyperlink ref="D4" r:id="rId17" location="8975k91/=19evlb8" xr:uid="{3EED6DB3-513A-4A9B-A132-2DF3D8EB3CFF}"/>
-    <hyperlink ref="D14" r:id="rId18" xr:uid="{1A45FFED-84A3-4DF1-94D9-66F1B415517E}"/>
+    <hyperlink ref="D16" r:id="rId18" xr:uid="{1A45FFED-84A3-4DF1-94D9-66F1B415517E}"/>
+    <hyperlink ref="D12" r:id="rId19" location="91251a158/=19n12mv" xr:uid="{4079C8D9-52E5-4341-A5A7-B95C96D3940B}"/>
+    <hyperlink ref="D24" r:id="rId20" location="8873a232/=19n144r" xr:uid="{AFCE556B-DA94-4A8E-A198-8CED990920DE}"/>
+    <hyperlink ref="D25" r:id="rId21" location="2866a84/=19n16ap" xr:uid="{4E70CB23-796A-465B-90F1-F9CCB1958E84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>